<commit_message>
Rel 1 on June 30 23
</commit_message>
<xml_diff>
--- a/article descriptions.xlsx
+++ b/article descriptions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/012c4a265263fc31/Environments/USArmy Project/armyyears/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="266" documentId="8_{43C26CEA-C0D9-47C8-8E60-8F0B531F8E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{487166AE-89B4-42BE-B25F-CC1E84D3269E}"/>
+  <xr:revisionPtr revIDLastSave="308" documentId="8_{43C26CEA-C0D9-47C8-8E60-8F0B531F8E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A74C6EF-B202-4880-A6F0-5A0F39C0193E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1CD9AE36-7E3E-44B6-9FC8-F093295C7A4C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
   <si>
     <t>Feature</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>First feature article US Army display of equipment Templehof airport open to the public</t>
+  </si>
+  <si>
+    <t>Feature article with picture -Boxing</t>
+  </si>
+  <si>
+    <t>Page</t>
   </si>
 </sst>
 </file>
@@ -166,12 +172,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -186,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -209,11 +221,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -302,17 +348,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0FABF3E7-80FE-4365-9468-712FFFB55D3C}" name="Table1" displayName="Table1" ref="A3:E27" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A3:E27" xr:uid="{0FABF3E7-80FE-4365-9468-712FFFB55D3C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E27">
-    <sortCondition ref="A3:A27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0FABF3E7-80FE-4365-9468-712FFFB55D3C}" name="Table1" displayName="Table1" ref="A3:F28" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A3:F28" xr:uid="{0FABF3E7-80FE-4365-9468-712FFFB55D3C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:F28">
+    <sortCondition ref="A3:A28"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{70082A82-68E4-4A30-86B7-19D164C8C13E}" name="Issue Date" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{C8EF89B3-4CF1-4611-9115-5BCE4C2D5845}" name="Feature" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{078888C5-09B1-4C73-84FB-0BD8CEF914F7}" name="Sports" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{45F16B5E-681F-4FC5-B09B-DD6E705229FC}" name="Feature Photo" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{9DD922C5-5E73-4FCA-A14F-805BD2AF3D84}" name="Briefs" dataDxfId="0"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{70082A82-68E4-4A30-86B7-19D164C8C13E}" name="Issue Date" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{C8EF89B3-4CF1-4611-9115-5BCE4C2D5845}" name="Feature" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{078888C5-09B1-4C73-84FB-0BD8CEF914F7}" name="Sports" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{45F16B5E-681F-4FC5-B09B-DD6E705229FC}" name="Feature Photo" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{9DD922C5-5E73-4FCA-A14F-805BD2AF3D84}" name="Briefs" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{904422D5-CE00-4188-AC36-FC8F0A48E7ED}" name="Page" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -615,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10BB4099-BF96-4A1C-8CF9-47412A266D7F}">
-  <dimension ref="A3:E36"/>
+  <dimension ref="A3:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,10 +673,10 @@
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.33203125" customWidth="1"/>
     <col min="3" max="3" width="31.21875" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="7"/>
+    <col min="5" max="5" width="14.21875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -645,8 +692,11 @@
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>25766</v>
       </c>
@@ -660,8 +710,11 @@
       <c r="E4" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>25913</v>
       </c>
@@ -675,8 +728,11 @@
       <c r="E5" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F5" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>25969</v>
       </c>
@@ -688,8 +744,11 @@
       <c r="E6" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>25976</v>
       </c>
@@ -701,8 +760,11 @@
       <c r="E7" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F7" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>25983</v>
       </c>
@@ -712,8 +774,11 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F8" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>25997</v>
       </c>
@@ -723,8 +788,11 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F9" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>26060</v>
       </c>
@@ -734,8 +802,11 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F10" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>26067</v>
       </c>
@@ -749,8 +820,11 @@
         <v>22</v>
       </c>
       <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F11" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>26074</v>
       </c>
@@ -760,8 +834,11 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F12" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>26081</v>
       </c>
@@ -771,8 +848,11 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F13" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>26109</v>
       </c>
@@ -784,8 +864,11 @@
         <v>19</v>
       </c>
       <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F14" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>26116</v>
       </c>
@@ -797,8 +880,11 @@
         <v>17</v>
       </c>
       <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>26123</v>
       </c>
@@ -808,8 +894,11 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F16" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>26130</v>
       </c>
@@ -821,130 +910,172 @@
         <v>14</v>
       </c>
       <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+      <c r="F17" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>26144</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
         <v>26165</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
-        <v>26172</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>26200</v>
+        <v>26172</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>26221</v>
+        <v>26200</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F21" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
+        <v>26221</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
         <v>26242</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5" t="s">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="E23" s="6"/>
+      <c r="F23" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
         <v>26263</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
-        <v>26270</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>3</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>26277</v>
+        <v>26270</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>26284</v>
+        <v>26277</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>26290</v>
+        <v>26284</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>26290</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
@@ -958,6 +1089,9 @@
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>